<commit_message>
- coexistence added  - test running  - some test fixes
</commit_message>
<xml_diff>
--- a/private/uploads/uploadFileTest.xlsx
+++ b/private/uploads/uploadFileTest.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natan.morote\Documents\accuarium-back\private\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C59C8E-56BC-4F51-836C-61ACE01226FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCF4108-3CF0-46F8-B2FF-C331DAD1AA46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="3384" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4275" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
     <sheet name="family" sheetId="2" r:id="rId2"/>
-    <sheet name="behavior" sheetId="3" r:id="rId3"/>
-    <sheet name="type" sheetId="4" r:id="rId4"/>
-    <sheet name="compatibility" sheetId="5" r:id="rId5"/>
-    <sheet name="hardness units" sheetId="6" r:id="rId6"/>
+    <sheet name="group" sheetId="8" r:id="rId3"/>
+    <sheet name="behavior" sheetId="3" r:id="rId4"/>
+    <sheet name="type" sheetId="4" r:id="rId5"/>
+    <sheet name="compatibility" sheetId="5" r:id="rId6"/>
+    <sheet name="hardness units" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="172">
   <si>
     <t>_id</t>
   </si>
@@ -107,12 +108,6 @@
     <t>maxKh</t>
   </si>
   <si>
-    <t>litersSpecimen</t>
-  </si>
-  <si>
-    <t>minTankLiters</t>
-  </si>
-  <si>
     <t>depth</t>
   </si>
   <si>
@@ -269,207 +264,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Anabántidos (Laberíntidos)</t>
-  </si>
-  <si>
-    <t>anabantoidei</t>
-  </si>
-  <si>
-    <t>Limpieza</t>
-  </si>
-  <si>
-    <t>Ancistrus</t>
-  </si>
-  <si>
-    <t>Comealgas</t>
-  </si>
-  <si>
-    <t>Anguiliformes</t>
-  </si>
-  <si>
-    <t>Cardumen</t>
-  </si>
-  <si>
-    <t>Bivalvos</t>
-  </si>
-  <si>
-    <t>Pequeño</t>
-  </si>
-  <si>
-    <t>Carácidos</t>
-  </si>
-  <si>
-    <t>Ornamental</t>
-  </si>
-  <si>
-    <t>Gasterópodos</t>
-  </si>
-  <si>
-    <t>Fondo</t>
-  </si>
-  <si>
-    <t>Cíclidos</t>
-  </si>
-  <si>
-    <t>Ciprinido</t>
-  </si>
-  <si>
-    <t>Crustáceos</t>
-  </si>
-  <si>
-    <t>Gymnotiformes</t>
-  </si>
-  <si>
-    <t>Loricaridos</t>
-  </si>
-  <si>
-    <t>Melanotaénidos</t>
-  </si>
-  <si>
-    <t>Osteoglósidos (arawana)</t>
-  </si>
-  <si>
-    <t>Poecílidos</t>
-  </si>
-  <si>
-    <t>Rajiformes</t>
-  </si>
-  <si>
-    <t>Silúridos</t>
-  </si>
-  <si>
-    <t>Tetraodontiformes (pez globo)</t>
-  </si>
-  <si>
-    <t>Balitóridos (Lonchas)</t>
-  </si>
-  <si>
-    <t>catostomidae</t>
-  </si>
-  <si>
-    <t>poeciliidae</t>
-  </si>
-  <si>
-    <t>Characids</t>
-  </si>
-  <si>
-    <t>characidae</t>
-  </si>
-  <si>
-    <t>gyrinocheilidae</t>
-  </si>
-  <si>
-    <t>Caracoles</t>
-  </si>
-  <si>
-    <t>amphilidae</t>
-  </si>
-  <si>
-    <t>Africano</t>
-  </si>
-  <si>
-    <t>Anguila</t>
-  </si>
-  <si>
-    <t>Arcoiris</t>
-  </si>
-  <si>
-    <t>Arowanas</t>
-  </si>
-  <si>
-    <t>Bettas</t>
-  </si>
-  <si>
-    <t>Botias</t>
-  </si>
-  <si>
-    <t>Corydoras</t>
-  </si>
-  <si>
-    <t>Danios</t>
-  </si>
-  <si>
-    <t>Discos</t>
-  </si>
-  <si>
-    <t>Escalares</t>
-  </si>
-  <si>
-    <t>Guppies</t>
-  </si>
-  <si>
-    <t>Killis</t>
-  </si>
-  <si>
-    <t>Labeos</t>
-  </si>
-  <si>
-    <t>Mollies</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t>Peces cocodrilo</t>
-  </si>
-  <si>
-    <t>Peces cuchillo</t>
-  </si>
-  <si>
-    <t>Peces globo</t>
-  </si>
-  <si>
-    <t>Peces sierra</t>
-  </si>
-  <si>
-    <t>Pirañas</t>
-  </si>
-  <si>
-    <t>Platies</t>
-  </si>
-  <si>
-    <t>Ramirezi</t>
-  </si>
-  <si>
-    <t>Rasboras</t>
-  </si>
-  <si>
-    <t>Rayas</t>
-  </si>
-  <si>
-    <t>Tetra</t>
-  </si>
-  <si>
-    <t>Xiphos</t>
-  </si>
-  <si>
-    <t>Barbos</t>
-  </si>
-  <si>
-    <t>Ciclidos Victoria</t>
-  </si>
-  <si>
-    <t>Ciclidos Malawi</t>
-  </si>
-  <si>
-    <t>Ciclidos Tanganika</t>
-  </si>
-  <si>
-    <t>Ciclidos asiáticos</t>
-  </si>
-  <si>
-    <t>Ciclidos norteamericanos</t>
-  </si>
-  <si>
-    <t>Ciclidos centroamericanos</t>
-  </si>
-  <si>
-    <t>Ciclidos sudamericanos</t>
-  </si>
-  <si>
-    <t>Cíclidos africanos fluviales</t>
-  </si>
-  <si>
     <t>Jumper</t>
   </si>
   <si>
@@ -588,13 +382,187 @@
   </si>
   <si>
     <t>gH</t>
+  </si>
+  <si>
+    <t>catostomids</t>
+  </si>
+  <si>
+    <t>cyprinids</t>
+  </si>
+  <si>
+    <t>characids</t>
+  </si>
+  <si>
+    <t>gyrinocheilids</t>
+  </si>
+  <si>
+    <t>loricarids</t>
+  </si>
+  <si>
+    <t>amphilids</t>
+  </si>
+  <si>
+    <t>cichlids</t>
+  </si>
+  <si>
+    <t>polycentrids</t>
+  </si>
+  <si>
+    <t>melanotaenids</t>
+  </si>
+  <si>
+    <t>osteoglosides</t>
+  </si>
+  <si>
+    <t>poecylids</t>
+  </si>
+  <si>
+    <t>silurids</t>
+  </si>
+  <si>
+    <t>tetraodontids</t>
+  </si>
+  <si>
+    <t>anablepids</t>
+  </si>
+  <si>
+    <t>fundulids</t>
+  </si>
+  <si>
+    <t>profundulus</t>
+  </si>
+  <si>
+    <t>eels</t>
+  </si>
+  <si>
+    <t>rainbow</t>
+  </si>
+  <si>
+    <t>arowanas</t>
+  </si>
+  <si>
+    <t>bettas</t>
+  </si>
+  <si>
+    <t>botias</t>
+  </si>
+  <si>
+    <t>corydoras</t>
+  </si>
+  <si>
+    <t>danios</t>
+  </si>
+  <si>
+    <t>discus</t>
+  </si>
+  <si>
+    <t>scalars</t>
+  </si>
+  <si>
+    <t>guppies</t>
+  </si>
+  <si>
+    <t>killis</t>
+  </si>
+  <si>
+    <t>labeos</t>
+  </si>
+  <si>
+    <t>mollies</t>
+  </si>
+  <si>
+    <t>oscar</t>
+  </si>
+  <si>
+    <t>crocodilefishes</t>
+  </si>
+  <si>
+    <t>knifefishes</t>
+  </si>
+  <si>
+    <t>blowfishes</t>
+  </si>
+  <si>
+    <t>sawfishes</t>
+  </si>
+  <si>
+    <t>piranhas</t>
+  </si>
+  <si>
+    <t>platies</t>
+  </si>
+  <si>
+    <t>rams</t>
+  </si>
+  <si>
+    <t>rasboras</t>
+  </si>
+  <si>
+    <t>stingrays</t>
+  </si>
+  <si>
+    <t>tetras</t>
+  </si>
+  <si>
+    <t>xiphos</t>
+  </si>
+  <si>
+    <t>barbs</t>
+  </si>
+  <si>
+    <t>south american cichlids</t>
+  </si>
+  <si>
+    <t>central american cichlids</t>
+  </si>
+  <si>
+    <t>north american cichlids</t>
+  </si>
+  <si>
+    <t>african rives cichlids</t>
+  </si>
+  <si>
+    <t>victoria cichlids</t>
+  </si>
+  <si>
+    <t>malawi cichlids</t>
+  </si>
+  <si>
+    <t>tanganika cichlids</t>
+  </si>
+  <si>
+    <t>catfishes</t>
+  </si>
+  <si>
+    <t>volumeSpecimen</t>
+  </si>
+  <si>
+    <t>minTankVoume</t>
+  </si>
+  <si>
+    <t>coupleCoexistence</t>
+  </si>
+  <si>
+    <t>onlyMascCoexistence</t>
+  </si>
+  <si>
+    <t>onlyFemCoexistence</t>
+  </si>
+  <si>
+    <t>haremCoexistence</t>
+  </si>
+  <si>
+    <t>inverseHaremCoexistence</t>
+  </si>
+  <si>
+    <t>indivCoexistence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,6 +613,13 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -660,7 +635,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -677,11 +652,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EAADB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -715,6 +705,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,11 +925,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomLeft" activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -946,16 +941,18 @@
     <col min="5" max="5" width="11.69921875" customWidth="1"/>
     <col min="6" max="6" width="25.09765625" customWidth="1"/>
     <col min="7" max="7" width="11.69921875" customWidth="1"/>
-    <col min="8" max="25" width="7.59765625" customWidth="1"/>
-    <col min="26" max="26" width="12.19921875" customWidth="1"/>
-    <col min="27" max="29" width="7.59765625" customWidth="1"/>
-    <col min="30" max="30" width="15" customWidth="1"/>
-    <col min="31" max="31" width="16.5" customWidth="1"/>
-    <col min="32" max="34" width="7.59765625" customWidth="1"/>
-    <col min="35" max="35" width="16.59765625" customWidth="1"/>
+    <col min="8" max="23" width="7.59765625" customWidth="1"/>
+    <col min="24" max="30" width="12" customWidth="1"/>
+    <col min="31" max="31" width="7.59765625" customWidth="1"/>
+    <col min="32" max="32" width="12.19921875" customWidth="1"/>
+    <col min="33" max="35" width="7.59765625" customWidth="1"/>
+    <col min="36" max="36" width="15" customWidth="1"/>
+    <col min="37" max="37" width="16.5" customWidth="1"/>
+    <col min="38" max="40" width="7.59765625" customWidth="1"/>
+    <col min="41" max="41" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,73 +1019,91 @@
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y1" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA1" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB1" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AL1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AM1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="K2" s="7">
         <v>4.5</v>
@@ -1107,7 +1122,7 @@
         <v>8</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>182</v>
+        <v>113</v>
       </c>
       <c r="R2" s="8">
         <v>5</v>
@@ -1116,7 +1131,7 @@
         <v>19</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>182</v>
+        <v>113</v>
       </c>
       <c r="U2" s="8">
         <v>2</v>
@@ -1130,43 +1145,61 @@
       <c r="X2" s="7">
         <v>100</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y2" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="Z2" s="8" t="s">
+    </row>
+    <row r="3" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="K3" s="7">
         <v>4.5</v>
@@ -1187,7 +1220,7 @@
         <v>7.5</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R3" s="8">
         <v>100</v>
@@ -1196,7 +1229,7 @@
         <v>150</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U3" s="10">
         <v>50</v>
@@ -1210,43 +1243,61 @@
       <c r="X3" s="7">
         <v>100</v>
       </c>
-      <c r="Y3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC3" s="7" t="s">
+      <c r="Y3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="K4" s="7">
         <v>4.5</v>
@@ -1267,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R4" s="8">
         <v>30</v>
@@ -1276,7 +1327,7 @@
         <v>60</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="U4" s="8">
         <v>15</v>
@@ -1290,43 +1341,61 @@
       <c r="X4" s="7">
         <v>100</v>
       </c>
-      <c r="Y4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC4" s="7" t="s">
+      <c r="Y4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="K5" s="7">
         <v>4.5</v>
@@ -1354,43 +1423,61 @@
       <c r="X5" s="7">
         <v>100</v>
       </c>
-      <c r="Y5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC5" s="7" t="s">
+      <c r="Y5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="K6" s="7">
         <v>4.5</v>
@@ -1418,43 +1505,61 @@
       <c r="X6" s="7">
         <v>100</v>
       </c>
-      <c r="Y6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC6" s="7" t="s">
+      <c r="Y6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="K7" s="7">
         <v>4.5</v>
@@ -1482,19 +1587,37 @@
       <c r="X7" s="7">
         <v>100</v>
       </c>
-      <c r="Y7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC7" s="7" t="s">
-        <v>58</v>
+      <c r="Y7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI7" s="7" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1514,7 +1637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" activeCellId="1" sqref="B17 D36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1527,12 +1652,12 @@
     <col min="11" max="26" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -1560,331 +1685,230 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>78</v>
-      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>80</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>82</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>84</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>86</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>88</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>73</v>
-      </c>
+      <c r="B10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>72</v>
-      </c>
+      <c r="B20" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="8" t="s">
-        <v>101</v>
-      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
-      <c r="C22" s="9" t="s">
-        <v>102</v>
-      </c>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>104</v>
-      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
     </row>
     <row r="24" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>106</v>
-      </c>
+      <c r="C24" s="9"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>108</v>
-      </c>
+      <c r="C25" s="8"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="7" t="s">
-        <v>110</v>
-      </c>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G28" s="7" t="s">
-        <v>111</v>
-      </c>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G29" s="7" t="s">
-        <v>112</v>
-      </c>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="7" t="s">
-        <v>113</v>
-      </c>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G31" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G32" s="7" t="s">
-        <v>115</v>
-      </c>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G33" s="7" t="s">
-        <v>116</v>
-      </c>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="7" t="s">
-        <v>117</v>
-      </c>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G35" s="7" t="s">
-        <v>118</v>
-      </c>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G36" s="7" t="s">
-        <v>119</v>
-      </c>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G37" s="7" t="s">
-        <v>120</v>
-      </c>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="7" t="s">
-        <v>121</v>
-      </c>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G39" s="7" t="s">
-        <v>122</v>
-      </c>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G40" s="7" t="s">
-        <v>123</v>
-      </c>
+      <c r="G40" s="7"/>
     </row>
     <row r="41" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G41" s="7" t="s">
-        <v>124</v>
-      </c>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G42" s="7" t="s">
-        <v>125</v>
-      </c>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G43" s="7" t="s">
-        <v>126</v>
-      </c>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G44" s="7" t="s">
-        <v>127</v>
-      </c>
+      <c r="G44" s="7"/>
     </row>
     <row r="45" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="7" t="s">
-        <v>128</v>
-      </c>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G46" s="7" t="s">
-        <v>129</v>
-      </c>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G47" s="7" t="s">
-        <v>130</v>
-      </c>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G48" s="7" t="s">
-        <v>131</v>
-      </c>
+      <c r="G48" s="7"/>
     </row>
     <row r="49" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G49" s="7" t="s">
-        <v>132</v>
-      </c>
+      <c r="G49" s="7"/>
     </row>
     <row r="50" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G50" s="7" t="s">
-        <v>133</v>
-      </c>
+      <c r="G50" s="7"/>
     </row>
     <row r="51" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G51" s="8" t="s">
-        <v>134</v>
-      </c>
+      <c r="G51" s="8"/>
     </row>
     <row r="52" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G52" s="8" t="s">
-        <v>135</v>
-      </c>
+      <c r="G52" s="8"/>
     </row>
     <row r="53" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G53" s="8" t="s">
-        <v>136</v>
-      </c>
+      <c r="G53" s="8"/>
     </row>
     <row r="54" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G54" s="8" t="s">
-        <v>137</v>
-      </c>
+      <c r="G54" s="8"/>
     </row>
     <row r="55" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G55" s="8" t="s">
-        <v>138</v>
-      </c>
+      <c r="G55" s="8"/>
     </row>
     <row r="56" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G56" s="8" t="s">
-        <v>139</v>
-      </c>
+      <c r="G56" s="8"/>
     </row>
     <row r="57" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G57" s="8" t="s">
-        <v>140</v>
-      </c>
+      <c r="G57" s="8"/>
     </row>
     <row r="58" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G58" s="8" t="s">
-        <v>141</v>
-      </c>
+      <c r="G58" s="8"/>
     </row>
     <row r="59" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G59" s="8" t="s">
-        <v>142</v>
-      </c>
+      <c r="G59" s="8"/>
     </row>
     <row r="60" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="7:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2829,168 +2853,403 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD524466-DF09-4E02-803E-07741E10F7DC}">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B2:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>146</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>149</v>
+        <v>80</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>155</v>
+        <v>86</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>156</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>158</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>159</v>
+        <v>90</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
-        <v>161</v>
+        <v>92</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>162</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>163</v>
+        <v>94</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>165</v>
+        <v>96</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>166</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>168</v>
+        <v>99</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>169</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>170</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>171</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>172</v>
+        <v>103</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>173</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>174</v>
+        <v>105</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>175</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>176</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2998,7 +3257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
@@ -3011,10 +3270,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -3043,17 +3302,17 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>177</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>178</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>179</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4058,7 +4317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4133,7 +4392,7 @@
         <v>badis badis</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="C2" s="17">
         <v>1</v>
@@ -4178,7 +4437,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="D3" s="17">
         <v>2</v>
@@ -4223,7 +4482,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="E4" s="17">
         <v>0</v>
@@ -4268,7 +4527,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="F5" s="17">
         <v>0</v>
@@ -4313,7 +4572,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="G6" s="17">
         <v>1</v>
@@ -4358,7 +4617,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="H7" s="17">
         <v>1</v>
@@ -4403,7 +4662,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="I8" s="17">
         <v>1</v>
@@ -4448,7 +4707,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="J9" s="17">
         <v>2</v>
@@ -4493,7 +4752,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="K10" s="17">
         <v>0</v>
@@ -4538,7 +4797,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="L11" s="17">
         <v>0</v>
@@ -4583,7 +4842,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="M12" s="8">
         <v>1</v>
@@ -4628,7 +4887,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -7850,7 +8109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7863,22 +8122,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>182</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>181</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- species model change - uploadFile adaptation - new behavior and family
</commit_message>
<xml_diff>
--- a/private/uploads/uploadFileTest.xlsx
+++ b/private/uploads/uploadFileTest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natan.morote\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natan.morote\Documents\accuarium-back\private\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3350FA-5BB7-4AA3-A27C-0820813DE72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3D9C65-8EB3-42E0-B879-7957E08670DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4275" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{7F1AADEE-A668-452D-89A2-922B8E27B743}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{0E3E47B5-D3B0-49C5-9B39-6967568475F7}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{7F1AADEE-A668-452D-89A2-922B8E27B743}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -245,9 +245,6 @@
     <t>multicolor</t>
   </si>
   <si>
-    <t>quite,shy</t>
-  </si>
-  <si>
     <t>Trichogaster lalia</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
   </si>
   <si>
     <t>opaline/blue/gold/choco gold/red gold/marvel</t>
-  </si>
-  <si>
-    <t>quite,shy,lover</t>
   </si>
   <si>
     <t>Trichopodus leerii</t>
@@ -983,6 +977,12 @@
   </si>
   <si>
     <t>mixedGroupCoexistence</t>
+  </si>
+  <si>
+    <t>quiet,shy</t>
+  </si>
+  <si>
+    <t>quiet,shy,lover</t>
   </si>
 </sst>
 </file>
@@ -1425,10 +1425,10 @@
   <dimension ref="A1:AN12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
+      <selection pane="bottomRight" activeCell="AK15" sqref="AK15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1554,7 +1554,7 @@
         <v>29</v>
       </c>
       <c r="AE1" s="29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>30</v>
@@ -1796,27 +1796,27 @@
       </c>
       <c r="AL3" s="8"/>
       <c r="AM3" s="10" t="s">
-        <v>63</v>
+        <v>307</v>
       </c>
       <c r="AN3" s="8"/>
     </row>
     <row r="4" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>39</v>
@@ -1903,32 +1903,32 @@
         <v>62</v>
       </c>
       <c r="AL4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM4" s="6" t="s">
-        <v>63</v>
+        <v>307</v>
       </c>
       <c r="AN4" s="4"/>
     </row>
     <row r="5" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="10">
         <v>1</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>39</v>
@@ -1958,7 +1958,7 @@
         <v>7.5</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R5" s="10">
         <v>36</v>
@@ -2012,35 +2012,35 @@
         <v>0</v>
       </c>
       <c r="AK5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL5" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="AL5" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="AM5" s="10" t="s">
-        <v>63</v>
+        <v>307</v>
       </c>
       <c r="AN5" s="8"/>
     </row>
     <row r="6" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="10">
         <v>1</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>39</v>
@@ -2124,33 +2124,33 @@
         <v>0</v>
       </c>
       <c r="AK6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AL6" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="AM6" s="10" t="s">
-        <v>83</v>
+        <v>308</v>
       </c>
       <c r="AN6" s="8"/>
     </row>
     <row r="7" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>39</v>
@@ -2230,33 +2230,33 @@
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8"/>
       <c r="AK7" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AL7" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AM7" s="8"/>
       <c r="AN7" s="8"/>
     </row>
     <row r="8" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="10">
         <v>1</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="G8" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>39</v>
@@ -2333,26 +2333,26 @@
         <v>45</v>
       </c>
       <c r="AL8" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AM8" s="8"/>
       <c r="AN8" s="8"/>
     </row>
     <row r="9" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="14" t="s">
+      <c r="E9" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -2384,7 +2384,7 @@
         <v>7.5</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R9" s="6">
         <v>90</v>
@@ -2438,35 +2438,35 @@
         <v>0</v>
       </c>
       <c r="AK9" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AL9" s="4"/>
       <c r="AM9" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AN9" s="4"/>
     </row>
     <row r="10" spans="1:40" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="14" t="s">
+      <c r="E10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>39</v>
@@ -2475,7 +2475,7 @@
         <v>40</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K10" s="4">
         <v>4</v>
@@ -2555,43 +2555,43 @@
         <v>62</v>
       </c>
       <c r="AL10" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AM10" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AN10" s="4"/>
     </row>
     <row r="11" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K11" s="8">
         <v>6</v>
@@ -2612,7 +2612,7 @@
         <v>7.5</v>
       </c>
       <c r="Q11" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R11" s="8">
         <v>18</v>
@@ -2655,7 +2655,7 @@
         <v>43</v>
       </c>
       <c r="AH11" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AI11" s="10">
         <v>0</v>
@@ -2664,42 +2664,42 @@
         <v>1</v>
       </c>
       <c r="AK11" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AL11" s="8"/>
       <c r="AM11" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AN11" s="8"/>
     </row>
     <row r="12" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B12" s="17">
         <v>1</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>39</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K12" s="8">
         <v>13</v>
@@ -2720,7 +2720,7 @@
         <v>7.5</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R12" s="8">
         <v>36</v>
@@ -2763,7 +2763,7 @@
         <v>43</v>
       </c>
       <c r="AH12" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AI12" s="8">
         <v>0</v>
@@ -2772,29 +2772,20 @@
         <v>1</v>
       </c>
       <c r="AK12" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AN12" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AN12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{0E3E47B5-D3B0-49C5-9B39-6967568475F7}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="B1:B1253" xr:uid="{E6949E5F-3912-4267-9A12-5C597011FC84}"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="241866329"/>
-        </ext>
-      </extLst>
-    </customSheetView>
     <customSheetView guid="{7F1AADEE-A668-452D-89A2-922B8E27B743}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AN1282" xr:uid="{4E18877C-ED4E-46EF-AFFE-6E3F6465D925}">
+      <autoFilter ref="A1:AN1282" xr:uid="{701EB8AF-C08C-4B92-B65B-300712403193}">
         <filterColumn colId="1">
           <filters>
             <filter val="1"/>
@@ -2804,6 +2795,15 @@
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1366459341"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{0E3E47B5-D3B0-49C5-9B39-6967568475F7}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="B1:B1253" xr:uid="{A3F2A5BD-0ADF-4608-AE5E-D02B6828CCBE}"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="241866329"/>
         </ext>
       </extLst>
     </customSheetView>
@@ -3066,7 +3066,7 @@
         <v>Helostoma temmincki</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" s="21">
         <v>1</v>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D3" s="21">
         <v>2</v>
@@ -3150,7 +3150,7 @@
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E4" s="21">
         <v>0</v>
@@ -3189,7 +3189,7 @@
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F5" s="21">
         <v>0</v>
@@ -3226,7 +3226,7 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G6" s="21">
         <v>1</v>
@@ -3261,7 +3261,7 @@
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H7" s="21">
         <v>1</v>
@@ -3294,7 +3294,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I8" s="21">
         <v>1</v>
@@ -3325,7 +3325,7 @@
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J9" s="21">
         <v>2</v>
@@ -3354,7 +3354,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K10" s="21">
         <v>0</v>
@@ -3381,7 +3381,7 @@
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
       <c r="K11" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L11" s="21">
         <v>0</v>
@@ -3406,7 +3406,7 @@
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M12" s="22">
         <v>1</v>
@@ -3429,7 +3429,7 @@
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3459,10 +3459,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -3491,15 +3491,15 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3507,220 +3507,220 @@
         <v>40</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C18" s="16"/>
     </row>
     <row r="19" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C26" s="26"/>
     </row>
     <row r="27" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="26" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C33" s="27"/>
     </row>
     <row r="34" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4719,10 +4719,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -4751,164 +4751,164 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="26" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C4" s="26"/>
       <c r="G4" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G10" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="G13" s="26" t="s">
         <v>233</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4916,281 +4916,281 @@
         <v>41</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="26" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="26" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G27" s="26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="26" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="26" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G36" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G37" s="26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="26" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="26" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="26" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G40" s="26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="26" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G41" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G43" s="26" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C44" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="G44" s="26" t="s">
         <v>251</v>
-      </c>
-      <c r="G44" s="26" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G46" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="26" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G47" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G48" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6166,10 +6166,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -6203,22 +6203,22 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7237,131 +7237,131 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="26" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="26" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="26" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="24" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
@@ -7369,7 +7369,7 @@
         <v>34</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
@@ -7377,31 +7377,31 @@
         <v>44</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="26" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="26" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="26" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -7427,7 +7427,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -7437,7 +7437,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -7473,7 +7473,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -7494,7 +7494,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -7504,7 +7504,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>